<commit_message>
change timezone change time of cronjobs
</commit_message>
<xml_diff>
--- a/src/mudules/assets/excel/Book1.xlsx
+++ b/src/mudules/assets/excel/Book1.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334BA770-9F40-4DF3-859C-8FE2A1CDFF7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E86E97AB-106E-49AC-862F-15280FA4D206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="2055" windowWidth="15375" windowHeight="7875" xr2:uid="{5822CE25-DC75-4245-8058-A692F45E15D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{5822CE25-DC75-4245-8058-A692F45E15D6}"/>
   </bookViews>
   <sheets>
     <sheet name="tổng quan" sheetId="1" r:id="rId1"/>
-    <sheet name="khách hàng" sheetId="3" r:id="rId2"/>
-    <sheet name="status" sheetId="2" r:id="rId3"/>
+    <sheet name="sản phẩm" sheetId="3" r:id="rId2"/>
+    <sheet name="Hướng dẫn sử dụng" sheetId="4" r:id="rId3"/>
+    <sheet name="status" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="deliveryStatusOptions">status!$A$2:$A$4</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>Hạn giao hàng</t>
   </si>
@@ -96,14 +97,26 @@
     <t>Đã thanh toán</t>
   </si>
   <si>
-    <t>Chưa thanh toán</t>
+    <t>HƯỚNG DẪN CÁCH SỬ DỤNG FILE ĐỂ IMPORT</t>
+  </si>
+  <si>
+    <t>Id Người mua hàng và Id của nhà cung cấp có thể copy ở bảng xem để dán vào</t>
+  </si>
+  <si>
+    <t>Tên sản phẩm</t>
+  </si>
+  <si>
+    <t>Khi nhập sản phẩm thì ứng với mỗi sản phẩm thì bắt đầu từ hàng số 5 và tiếp tục với các hàng sau cho các sản phẩm tương ứng (ví dụ Sản phẩm thứ 2 sẽ bắt đầu viết ở hàng số 6)</t>
+  </si>
+  <si>
+    <t>Ở sheet sản phẩm, có thể copy Id và Tên Sản phẩm trong mục Sản phẩm của nhà cung cấp đó để paste vào</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -115,6 +128,13 @@
       <color theme="1"/>
       <name val="Source Sans Pro"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,10 +157,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,7 +478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B488B0-29E6-4392-B86D-1FEB0014ED73}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -466,8 +487,8 @@
     <col min="1" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="19.77734375" customWidth="1"/>
-    <col min="5" max="5" width="22.88671875" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="26.77734375" customWidth="1"/>
+    <col min="6" max="6" width="23.109375" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" customWidth="1"/>
     <col min="8" max="8" width="14.88671875" customWidth="1"/>
   </cols>
@@ -501,15 +522,7 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
+      <c r="H2" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -521,51 +534,60 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B3936B-D4A4-42A4-98B5-C6CCC2A8661F}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="1" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -574,11 +596,50 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D091915C-546E-4B48-9345-993BA05F8787}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView zoomScale="59" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D87C93A7-5974-4F01-A023-F783018D6920}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>

</xml_diff>